<commit_message>
Se modifica actividad para ejercicios de excel
</commit_message>
<xml_diff>
--- a/2_2/activity.xlsx
+++ b/2_2/activity.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\won_m\OneDrive\Documentos\EDUCEM\2023-1\BACHILLERATO\activities\2_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EF8FD7B-8C5D-41A8-A90F-10771674A470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760EBCE4-80E2-4253-9324-D6039A43EBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C157B75A-14D9-468C-8966-3A5D037493EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>Alumno</t>
   </si>
@@ -112,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,13 +147,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +173,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -181,11 +203,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,11 +230,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +556,7 @@
   <dimension ref="B3:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,34 +707,34 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -702,160 +743,144 @@
         <v>21</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="5">
-        <v>9.5</v>
-      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="4">
-        <v>7.625</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="4">
-        <v>7.333333333333333</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>